<commit_message>
TN met feb nulmetingen aangemaakt
</commit_message>
<xml_diff>
--- a/Scriptie - Experiment resultaten.xlsx
+++ b/Scriptie - Experiment resultaten.xlsx
@@ -59,9 +59,9 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="3">
-    <numFmt numFmtId="165" formatCode="0.00000000"/>
-    <numFmt numFmtId="175" formatCode="0.00000000000000"/>
-    <numFmt numFmtId="176" formatCode="0.000000000000000"/>
+    <numFmt numFmtId="164" formatCode="0.00000000"/>
+    <numFmt numFmtId="165" formatCode="0.00000000000000"/>
+    <numFmt numFmtId="166" formatCode="0.000000000000000"/>
   </numFmts>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
@@ -94,10 +94,10 @@
   </cellStyleXfs>
   <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="175" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standaard" xfId="0" builtinId="0"/>
@@ -7984,8 +7984,8 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="64071936"/>
-        <c:axId val="64073728"/>
+        <c:axId val="123989376"/>
+        <c:axId val="123991552"/>
       </c:lineChart>
       <c:lineChart>
         <c:grouping val="standard"/>
@@ -9618,11 +9618,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="164220288"/>
-        <c:axId val="164178560"/>
+        <c:axId val="123996032"/>
+        <c:axId val="123993472"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="64071936"/>
+        <c:axId val="123989376"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -9655,14 +9655,13 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="out"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="64073728"/>
+        <c:crossAx val="123991552"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -9672,7 +9671,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="64073728"/>
+        <c:axId val="123991552"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -9705,19 +9704,18 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="64071936"/>
+        <c:crossAx val="123989376"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="164178560"/>
+        <c:axId val="123993472"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -9739,20 +9737,18 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="out"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="164220288"/>
+        <c:crossAx val="123996032"/>
         <c:crosses val="max"/>
         <c:crossBetween val="between"/>
         <c:dispUnits>
           <c:builtInUnit val="millions"/>
           <c:dispUnitsLbl>
-            <c:layout/>
             <c:tx>
               <c:rich>
                 <a:bodyPr rot="0" vert="horz"/>
@@ -9772,7 +9768,7 @@
         </c:dispUnits>
       </c:valAx>
       <c:catAx>
-        <c:axId val="164220288"/>
+        <c:axId val="123996032"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -9782,7 +9778,8 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="164178560"/>
+        <c:crossAx val="123993472"/>
+        <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
@@ -9791,7 +9788,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -14465,9 +14461,9 @@
           <c:spPr>
             <a:ln>
               <a:solidFill>
-                <a:schemeClr val="tx1">
+                <a:srgbClr val="00B0F0">
                   <a:alpha val="25000"/>
-                </a:schemeClr>
+                </a:srgbClr>
               </a:solidFill>
             </a:ln>
           </c:spPr>
@@ -19999,7 +19995,7 @@
           <c:spPr>
             <a:ln>
               <a:solidFill>
-                <a:schemeClr val="tx1"/>
+                <a:srgbClr val="00B0F0"/>
               </a:solidFill>
             </a:ln>
           </c:spPr>
@@ -21608,8 +21604,8 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="170165376"/>
-        <c:axId val="170167296"/>
+        <c:axId val="95461376"/>
+        <c:axId val="95463296"/>
       </c:lineChart>
       <c:lineChart>
         <c:grouping val="standard"/>
@@ -21649,11 +21645,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="164309248"/>
-        <c:axId val="164223616"/>
+        <c:axId val="95471872"/>
+        <c:axId val="95469952"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="170165376"/>
+        <c:axId val="95461376"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -21693,7 +21689,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="out"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="170167296"/>
+        <c:crossAx val="95463296"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -21703,7 +21699,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="170167296"/>
+        <c:axId val="95463296"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -21743,7 +21739,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="170165376"/>
+        <c:crossAx val="95461376"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
         <c:dispUnits>
@@ -21769,7 +21765,7 @@
         </c:dispUnits>
       </c:valAx>
       <c:valAx>
-        <c:axId val="164223616"/>
+        <c:axId val="95469952"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="0.55000000000000004"/>
@@ -21811,14 +21807,14 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="164309248"/>
+        <c:crossAx val="95471872"/>
         <c:crosses val="max"/>
         <c:crossBetween val="between"/>
         <c:majorUnit val="0.1"/>
         <c:minorUnit val="2.0000000000000004E-2"/>
       </c:valAx>
       <c:catAx>
-        <c:axId val="164309248"/>
+        <c:axId val="95471872"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -21827,7 +21823,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="164223616"/>
+        <c:crossAx val="95469952"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>

</xml_diff>

<commit_message>
Scriptie - Voorwoord + Managementsamenvatting + Inleiding geschreven
</commit_message>
<xml_diff>
--- a/Scriptie - Experiment resultaten.xlsx
+++ b/Scriptie - Experiment resultaten.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="-150" yWindow="-480" windowWidth="29100" windowHeight="13455"/>
+    <workbookView xWindow="-150" yWindow="-420" windowWidth="29100" windowHeight="13395"/>
   </bookViews>
   <sheets>
     <sheet name="Fitnesses &amp; Outputs" sheetId="1" r:id="rId1"/>
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="29">
   <si>
     <t>Generatie</t>
   </si>
@@ -55,15 +55,6 @@
     <t>Sinus ovenbuffers na</t>
   </si>
   <si>
-    <t>Nulmeting Sinus Fitness</t>
-  </si>
-  <si>
-    <t>Nulmeting Sinus Gem. Fitness</t>
-  </si>
-  <si>
-    <t>Nulmeting Sinus Output</t>
-  </si>
-  <si>
     <t>Nulmeting Sinus persbuffers na</t>
   </si>
   <si>
@@ -79,22 +70,40 @@
     <t>Nulmeting --&gt;</t>
   </si>
   <si>
-    <t>Lineair persbuffers na</t>
+    <t>5% synapses Fitness</t>
   </si>
   <si>
-    <t>Lineair persbuffers voor</t>
+    <t>5% synapses Gem. Fitness</t>
   </si>
   <si>
-    <t>Lineair ovenbuffers na</t>
+    <t>5% synapses Output</t>
   </si>
   <si>
-    <t>Nulmeting Lineair Fitness</t>
+    <t>100% synapses Fitness</t>
   </si>
   <si>
-    <t>Nulmeting Lineair Gem. Fitness</t>
+    <t>100% synases Gem. Fitness</t>
   </si>
   <si>
-    <t>Nulmeting Lineair Output</t>
+    <t>100% synapses Output</t>
+  </si>
+  <si>
+    <t>5% synapses persbuffers na</t>
+  </si>
+  <si>
+    <t>5% synapses persbuffers voor</t>
+  </si>
+  <si>
+    <t>5% synapses ovenbuffers na</t>
+  </si>
+  <si>
+    <t>100% synapses persbuffers na</t>
+  </si>
+  <si>
+    <t>100% synapses persbuffers voor</t>
+  </si>
+  <si>
+    <t>100% synapses ovenbuffers na</t>
   </si>
 </sst>
 </file>
@@ -8135,8 +8144,8 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="39552512"/>
-        <c:axId val="39554432"/>
+        <c:axId val="143058048"/>
+        <c:axId val="143059968"/>
       </c:lineChart>
       <c:lineChart>
         <c:grouping val="standard"/>
@@ -9817,11 +9826,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="39575552"/>
-        <c:axId val="39560704"/>
+        <c:axId val="85990784"/>
+        <c:axId val="85988480"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="39552512"/>
+        <c:axId val="143058048"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -9861,7 +9870,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="out"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="39554432"/>
+        <c:crossAx val="143059968"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -9871,7 +9880,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="39554432"/>
+        <c:axId val="143059968"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -9911,12 +9920,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="39552512"/>
+        <c:crossAx val="143058048"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="39560704"/>
+        <c:axId val="85988480"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -9957,7 +9966,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="out"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="39575552"/>
+        <c:crossAx val="85990784"/>
         <c:crosses val="max"/>
         <c:crossBetween val="between"/>
         <c:dispUnits>
@@ -9978,7 +9987,7 @@
         </c:dispUnits>
       </c:valAx>
       <c:catAx>
-        <c:axId val="39575552"/>
+        <c:axId val="85990784"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -9988,7 +9997,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="39560704"/>
+        <c:crossAx val="85988480"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -10061,7 +10070,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Nulmeting Sinus Fitness</c:v>
+                  <c:v>5% synapses Fitness</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -10903,7 +10912,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Nulmeting Sinus Gem. Fitness</c:v>
+                  <c:v>5% synapses Gem. Fitness</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -11285,7 +11294,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Nulmeting Lineair Fitness</c:v>
+                  <c:v>100% synapses Fitness</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -11310,25 +11319,7 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.1051189</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>0.1959719</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>0.1959719</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>0.1966253</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>0.19916629999999999</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>0.199181</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>0.20088200000000001</c:v>
+                  <c:v>0.22023010000000001</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -11344,7 +11335,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Nulmeting Lineair Gem. Fitness</c:v>
+                  <c:v>100% synases Gem. Fitness</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -11371,25 +11362,7 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>9.3060959999999998E-2</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>9.6589019999999998E-2</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>9.6282000000000006E-2</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>0.1174762</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>0.12069439999999999</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>0.12671389999999999</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>0.12660060000000001</c:v>
+                  <c:v>0.21034140000000001</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -11406,8 +11379,8 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="39882752"/>
-        <c:axId val="39884672"/>
+        <c:axId val="86036864"/>
+        <c:axId val="86038784"/>
       </c:lineChart>
       <c:lineChart>
         <c:grouping val="standard"/>
@@ -11421,7 +11394,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Nulmeting Sinus Output</c:v>
+                  <c:v>5% synapses Output</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -11429,9 +11402,7 @@
           <c:spPr>
             <a:ln>
               <a:solidFill>
-                <a:srgbClr val="F79646">
-                  <a:alpha val="50000"/>
-                </a:srgbClr>
+                <a:srgbClr val="F79646"/>
               </a:solidFill>
               <a:prstDash val="dash"/>
             </a:ln>
@@ -11804,7 +11775,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Nulmeting Lineair Output</c:v>
+                  <c:v>100% synapses Output</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -11812,9 +11783,7 @@
           <c:spPr>
             <a:ln>
               <a:solidFill>
-                <a:srgbClr val="FF0000">
-                  <a:alpha val="50000"/>
-                </a:srgbClr>
+                <a:srgbClr val="FF0000"/>
               </a:solidFill>
               <a:prstDash val="dash"/>
             </a:ln>
@@ -11832,25 +11801,7 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>29372000</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>54760000</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>54760000</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>54943000</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>55654000</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>55658000</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>56134000</c:v>
+                  <c:v>61540000</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -11867,11 +11818,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="39897344"/>
-        <c:axId val="39895040"/>
+        <c:axId val="96213632"/>
+        <c:axId val="96211328"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="39882752"/>
+        <c:axId val="86036864"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -11911,7 +11862,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="out"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="39884672"/>
+        <c:crossAx val="86038784"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -11921,7 +11872,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="39884672"/>
+        <c:axId val="86038784"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -11961,12 +11912,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="39882752"/>
+        <c:crossAx val="86036864"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="39895040"/>
+        <c:axId val="96211328"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -12007,7 +11958,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="out"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="39897344"/>
+        <c:crossAx val="96213632"/>
         <c:crosses val="max"/>
         <c:crossBetween val="between"/>
         <c:dispUnits>
@@ -12018,7 +11969,7 @@
         </c:dispUnits>
       </c:valAx>
       <c:catAx>
-        <c:axId val="39897344"/>
+        <c:axId val="96213632"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -12028,7 +11979,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="39895040"/>
+        <c:crossAx val="96211328"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -23999,8 +23950,8 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="163234560"/>
-        <c:axId val="163236480"/>
+        <c:axId val="97870592"/>
+        <c:axId val="97872512"/>
       </c:lineChart>
       <c:lineChart>
         <c:grouping val="standard"/>
@@ -24061,11 +24012,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="100666368"/>
-        <c:axId val="100664448"/>
+        <c:axId val="97889280"/>
+        <c:axId val="97887360"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="163234560"/>
+        <c:axId val="97870592"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -24105,7 +24056,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="out"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="163236480"/>
+        <c:crossAx val="97872512"/>
         <c:crosses val="autoZero"/>
         <c:auto val="0"/>
         <c:lblAlgn val="ctr"/>
@@ -24115,7 +24066,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="163236480"/>
+        <c:axId val="97872512"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -24155,7 +24106,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="out"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="163234560"/>
+        <c:crossAx val="97870592"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
         <c:dispUnits>
@@ -24181,7 +24132,7 @@
         </c:dispUnits>
       </c:valAx>
       <c:valAx>
-        <c:axId val="100664448"/>
+        <c:axId val="97887360"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="2.29577009361005"/>
@@ -24224,14 +24175,14 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="100666368"/>
+        <c:crossAx val="97889280"/>
         <c:crosses val="max"/>
         <c:crossBetween val="between"/>
         <c:majorUnit val="0.25"/>
         <c:minorUnit val="5.000000000000001E-2"/>
       </c:valAx>
       <c:catAx>
-        <c:axId val="100666368"/>
+        <c:axId val="97889280"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -24240,7 +24191,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="100664448"/>
+        <c:crossAx val="97887360"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -24299,7 +24250,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Sinus persbuffers na</c:v>
+                  <c:v>5% synapses persbuffers na</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -25143,7 +25094,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Sinus persbuffers voor</c:v>
+                  <c:v>5% synapses persbuffers voor</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -25987,7 +25938,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Sinus ovenbuffers na</c:v>
+                  <c:v>5% synapses ovenbuffers na</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -26831,7 +26782,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Lineair persbuffers na</c:v>
+                  <c:v>100% synapses persbuffers na</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -26853,28 +26804,10 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="151"/>
                 <c:pt idx="0">
-                  <c:v>17000</c:v>
+                  <c:v>2324000</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>17000</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>406000</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>406000</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>406000</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>406000</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>406000</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>406000</c:v>
+                  <c:v>2362000</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -26890,7 +26823,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Lineair persbuffers voor</c:v>
+                  <c:v>100% synapses persbuffers voor</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -26912,28 +26845,10 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="151"/>
                 <c:pt idx="0">
-                  <c:v>17000</c:v>
+                  <c:v>1773000</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>17000</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>17000</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>17000</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>17000</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>17000</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>17000</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>17000</c:v>
+                  <c:v>1884000</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -26949,7 +26864,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Lineair ovenbuffers na</c:v>
+                  <c:v>100% synapses ovenbuffers na</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -26971,28 +26886,10 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="151"/>
                 <c:pt idx="0">
-                  <c:v>1076000</c:v>
+                  <c:v>545000</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1076000</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>2901000</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>2901000</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>3306000</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>4279000</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>4189000</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>4871000</c:v>
+                  <c:v>506000</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -27009,8 +26906,8 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="100700928"/>
-        <c:axId val="100702848"/>
+        <c:axId val="98603776"/>
+        <c:axId val="98605696"/>
       </c:lineChart>
       <c:lineChart>
         <c:grouping val="standard"/>
@@ -27071,11 +26968,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="100719616"/>
-        <c:axId val="100717696"/>
+        <c:axId val="98618368"/>
+        <c:axId val="98616448"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="100700928"/>
+        <c:axId val="98603776"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -27115,7 +27012,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="out"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="100702848"/>
+        <c:crossAx val="98605696"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -27125,7 +27022,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="100702848"/>
+        <c:axId val="98605696"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -27165,7 +27062,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="out"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="100700928"/>
+        <c:crossAx val="98603776"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
         <c:dispUnits>
@@ -27191,7 +27088,7 @@
         </c:dispUnits>
       </c:valAx>
       <c:valAx>
-        <c:axId val="100717696"/>
+        <c:axId val="98616448"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="4.1323861684980878"/>
@@ -27234,14 +27131,14 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="100719616"/>
+        <c:crossAx val="98618368"/>
         <c:crosses val="max"/>
         <c:crossBetween val="between"/>
         <c:majorUnit val="0.5"/>
         <c:minorUnit val="0.25"/>
       </c:valAx>
       <c:catAx>
-        <c:axId val="100719616"/>
+        <c:axId val="98618368"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -27250,7 +27147,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="100717696"/>
+        <c:crossAx val="98616448"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -39208,8 +39105,8 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="101643776"/>
-        <c:axId val="101645696"/>
+        <c:axId val="98010624"/>
+        <c:axId val="98012544"/>
       </c:lineChart>
       <c:lineChart>
         <c:grouping val="standard"/>
@@ -39270,11 +39167,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="100806656"/>
-        <c:axId val="100800384"/>
+        <c:axId val="98033664"/>
+        <c:axId val="98019200"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="101643776"/>
+        <c:axId val="98010624"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -39307,14 +39204,13 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="#,##0" sourceLinked="0"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="out"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="101645696"/>
+        <c:crossAx val="98012544"/>
         <c:crosses val="autoZero"/>
         <c:auto val="0"/>
         <c:lblAlgn val="ctr"/>
@@ -39324,7 +39220,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="101645696"/>
+        <c:axId val="98012544"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -39357,20 +39253,18 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="101643776"/>
+        <c:crossAx val="98010624"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
         <c:dispUnits>
           <c:builtInUnit val="millions"/>
           <c:dispUnitsLbl>
-            <c:layout/>
             <c:tx>
               <c:rich>
                 <a:bodyPr rot="0" vert="horz"/>
@@ -39390,7 +39284,7 @@
         </c:dispUnits>
       </c:valAx>
       <c:valAx>
-        <c:axId val="100800384"/>
+        <c:axId val="98019200"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="0.55098482246641212"/>
@@ -39425,21 +39319,20 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="100806656"/>
+        <c:crossAx val="98033664"/>
         <c:crosses val="max"/>
         <c:crossBetween val="between"/>
         <c:majorUnit val="0.1"/>
         <c:minorUnit val="2.0000000000000004E-2"/>
       </c:valAx>
       <c:catAx>
-        <c:axId val="100806656"/>
+        <c:axId val="98033664"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -39448,7 +39341,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="100800384"/>
+        <c:crossAx val="98019200"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -39458,7 +39351,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -41365,8 +41257,8 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="100846208"/>
-        <c:axId val="100856576"/>
+        <c:axId val="98397184"/>
+        <c:axId val="98407552"/>
       </c:lineChart>
       <c:lineChart>
         <c:grouping val="standard"/>
@@ -41427,11 +41319,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="101655680"/>
-        <c:axId val="100858880"/>
+        <c:axId val="98416128"/>
+        <c:axId val="98409856"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="100846208"/>
+        <c:axId val="98397184"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -41464,14 +41356,13 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="#,##0" sourceLinked="0"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="out"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="100856576"/>
+        <c:crossAx val="98407552"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -41481,7 +41372,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="100856576"/>
+        <c:axId val="98407552"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -41514,20 +41405,18 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="100846208"/>
+        <c:crossAx val="98397184"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
         <c:dispUnits>
           <c:builtInUnit val="millions"/>
           <c:dispUnitsLbl>
-            <c:layout/>
             <c:tx>
               <c:rich>
                 <a:bodyPr rot="0" vert="horz"/>
@@ -41547,7 +41436,7 @@
         </c:dispUnits>
       </c:valAx>
       <c:valAx>
-        <c:axId val="100858880"/>
+        <c:axId val="98409856"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="0.55098482246641212"/>
@@ -41582,21 +41471,20 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="101655680"/>
+        <c:crossAx val="98416128"/>
         <c:crosses val="max"/>
         <c:crossBetween val="between"/>
         <c:majorUnit val="0.1"/>
         <c:minorUnit val="2.0000000000000004E-2"/>
       </c:valAx>
       <c:catAx>
-        <c:axId val="101655680"/>
+        <c:axId val="98416128"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -41605,7 +41493,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="100858880"/>
+        <c:crossAx val="98409856"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -41615,7 +41503,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -41670,15 +41557,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>9</xdr:col>
-      <xdr:colOff>476250</xdr:colOff>
-      <xdr:row>7</xdr:row>
-      <xdr:rowOff>19050</xdr:rowOff>
+      <xdr:colOff>161925</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>180975</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>20</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>295275</xdr:colOff>
       <xdr:row>30</xdr:row>
-      <xdr:rowOff>152400</xdr:rowOff>
+      <xdr:rowOff>123825</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -42408,7 +42295,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:M378"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
       <selection activeCell="O2" sqref="O2"/>
     </sheetView>
   </sheetViews>
@@ -42420,12 +42307,12 @@
     <col min="5" max="5" width="12.42578125" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="17.85546875" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="12.42578125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="22.7109375" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="28" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="22.7109375" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="24" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="29.28515625" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="24" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="19" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="24.28515625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="19" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="21" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="25.140625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="21" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="2:13" x14ac:dyDescent="0.25">
@@ -42448,22 +42335,22 @@
         <v>5</v>
       </c>
       <c r="H2" t="s">
-        <v>12</v>
+        <v>17</v>
       </c>
       <c r="I2" t="s">
-        <v>13</v>
+        <v>18</v>
       </c>
       <c r="J2" t="s">
-        <v>14</v>
+        <v>19</v>
       </c>
       <c r="K2" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="L2" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="M2" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
     </row>
     <row r="3" spans="2:13" x14ac:dyDescent="0.25">
@@ -42533,13 +42420,13 @@
         <v>32333000</v>
       </c>
       <c r="K4">
-        <v>0.1051189</v>
+        <v>0.22023010000000001</v>
       </c>
       <c r="L4">
-        <v>9.3060959999999998E-2</v>
+        <v>0.21034140000000001</v>
       </c>
       <c r="M4">
-        <v>29372000</v>
+        <v>61540000</v>
       </c>
     </row>
     <row r="5" spans="2:13" x14ac:dyDescent="0.25">
@@ -42570,15 +42457,6 @@
       <c r="J5">
         <v>32946000</v>
       </c>
-      <c r="K5">
-        <v>0.1959719</v>
-      </c>
-      <c r="L5">
-        <v>9.6589019999999998E-2</v>
-      </c>
-      <c r="M5">
-        <v>54760000</v>
-      </c>
     </row>
     <row r="6" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B6">
@@ -42608,15 +42486,6 @@
       <c r="J6">
         <v>32946000</v>
       </c>
-      <c r="K6">
-        <v>0.1959719</v>
-      </c>
-      <c r="L6">
-        <v>9.6282000000000006E-2</v>
-      </c>
-      <c r="M6">
-        <v>54760000</v>
-      </c>
     </row>
     <row r="7" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B7">
@@ -42646,15 +42515,6 @@
       <c r="J7">
         <v>32946000</v>
       </c>
-      <c r="K7">
-        <v>0.1966253</v>
-      </c>
-      <c r="L7">
-        <v>0.1174762</v>
-      </c>
-      <c r="M7">
-        <v>54943000</v>
-      </c>
     </row>
     <row r="8" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B8">
@@ -42684,15 +42544,6 @@
       <c r="J8">
         <v>32946000</v>
       </c>
-      <c r="K8">
-        <v>0.19916629999999999</v>
-      </c>
-      <c r="L8">
-        <v>0.12069439999999999</v>
-      </c>
-      <c r="M8">
-        <v>55654000</v>
-      </c>
     </row>
     <row r="9" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B9">
@@ -42722,15 +42573,6 @@
       <c r="J9">
         <v>32971000</v>
       </c>
-      <c r="K9">
-        <v>0.199181</v>
-      </c>
-      <c r="L9">
-        <v>0.12671389999999999</v>
-      </c>
-      <c r="M9">
-        <v>55658000</v>
-      </c>
     </row>
     <row r="10" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B10">
@@ -42759,15 +42601,6 @@
       </c>
       <c r="J10">
         <v>32971000</v>
-      </c>
-      <c r="K10">
-        <v>0.20088200000000001</v>
-      </c>
-      <c r="L10">
-        <v>0.12660060000000001</v>
-      </c>
-      <c r="M10">
-        <v>56134000</v>
       </c>
     </row>
     <row r="11" spans="2:13" x14ac:dyDescent="0.25">
@@ -49208,18 +49041,18 @@
     <col min="6" max="6" width="24.5703125" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="25.7109375" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="24.5703125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="29.42578125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="31.42578125" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="24.7109375" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="20.5703125" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="22.5703125" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="21.140625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="25.85546875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="27.7109375" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="26.42578125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="27.85546875" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="29.85546875" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="28.42578125" bestFit="1" customWidth="1"/>
     <col min="16" max="16" width="17.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="2:17" x14ac:dyDescent="0.25">
       <c r="I1" s="6" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
     </row>
     <row r="2" spans="2:17" x14ac:dyDescent="0.25">
@@ -49245,25 +49078,25 @@
         <v>11</v>
       </c>
       <c r="I2" t="s">
-        <v>9</v>
+        <v>23</v>
       </c>
       <c r="J2" t="s">
-        <v>10</v>
+        <v>24</v>
       </c>
       <c r="K2" t="s">
-        <v>11</v>
+        <v>25</v>
       </c>
       <c r="L2" t="s">
-        <v>20</v>
+        <v>26</v>
       </c>
       <c r="M2" t="s">
-        <v>21</v>
+        <v>27</v>
       </c>
       <c r="N2" t="s">
-        <v>22</v>
+        <v>28</v>
       </c>
       <c r="P2" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
     </row>
     <row r="3" spans="2:17" x14ac:dyDescent="0.25">
@@ -49298,13 +49131,13 @@
         <v>7460000</v>
       </c>
       <c r="L3">
-        <v>17000</v>
+        <v>2324000</v>
       </c>
       <c r="M3">
-        <v>17000</v>
+        <v>1773000</v>
       </c>
       <c r="N3">
-        <v>1076000</v>
+        <v>545000</v>
       </c>
       <c r="P3">
         <f>P9/6*0</f>
@@ -49347,13 +49180,13 @@
         <v>7916000</v>
       </c>
       <c r="L4">
-        <v>17000</v>
+        <v>2362000</v>
       </c>
       <c r="M4">
-        <v>17000</v>
+        <v>1884000</v>
       </c>
       <c r="N4">
-        <v>1076000</v>
+        <v>506000</v>
       </c>
       <c r="P4" s="4">
         <f>P9/6*1</f>
@@ -49395,15 +49228,6 @@
       <c r="K5">
         <v>10860000</v>
       </c>
-      <c r="L5">
-        <v>406000</v>
-      </c>
-      <c r="M5">
-        <v>17000</v>
-      </c>
-      <c r="N5">
-        <v>2901000</v>
-      </c>
       <c r="P5" s="3">
         <f>P9/6*2</f>
         <v>1.3774620561660298</v>
@@ -49444,15 +49268,6 @@
       <c r="K6">
         <v>10860000</v>
       </c>
-      <c r="L6">
-        <v>406000</v>
-      </c>
-      <c r="M6">
-        <v>17000</v>
-      </c>
-      <c r="N6">
-        <v>2901000</v>
-      </c>
       <c r="P6" s="3">
         <f>P9/6*3</f>
         <v>2.0661930842490448</v>
@@ -49493,15 +49308,6 @@
       <c r="K7">
         <v>10860000</v>
       </c>
-      <c r="L7">
-        <v>406000</v>
-      </c>
-      <c r="M7">
-        <v>17000</v>
-      </c>
-      <c r="N7">
-        <v>3306000</v>
-      </c>
       <c r="P7" s="3">
         <f>P9/6*4</f>
         <v>2.7549241123320596</v>
@@ -49542,15 +49348,6 @@
       <c r="K8">
         <v>10860000</v>
       </c>
-      <c r="L8">
-        <v>406000</v>
-      </c>
-      <c r="M8">
-        <v>17000</v>
-      </c>
-      <c r="N8">
-        <v>4279000</v>
-      </c>
       <c r="P8" s="3">
         <f>P9/6*5</f>
         <v>3.4436551404150744</v>
@@ -49591,15 +49388,6 @@
       <c r="K9">
         <v>13198000</v>
       </c>
-      <c r="L9">
-        <v>406000</v>
-      </c>
-      <c r="M9">
-        <v>17000</v>
-      </c>
-      <c r="N9">
-        <v>4189000</v>
-      </c>
       <c r="P9" s="3">
         <v>4.1323861684980896</v>
       </c>
@@ -49638,15 +49426,6 @@
       </c>
       <c r="K10">
         <v>13198000</v>
-      </c>
-      <c r="L10">
-        <v>406000</v>
-      </c>
-      <c r="M10">
-        <v>17000</v>
-      </c>
-      <c r="N10">
-        <v>4871000</v>
       </c>
     </row>
     <row r="11" spans="2:17" x14ac:dyDescent="0.25">
@@ -57588,16 +57367,16 @@
         <v>11</v>
       </c>
       <c r="I2" t="s">
+        <v>12</v>
+      </c>
+      <c r="J2" t="s">
+        <v>13</v>
+      </c>
+      <c r="K2" t="s">
+        <v>14</v>
+      </c>
+      <c r="M2" t="s">
         <v>15</v>
-      </c>
-      <c r="J2" t="s">
-        <v>16</v>
-      </c>
-      <c r="K2" t="s">
-        <v>17</v>
-      </c>
-      <c r="M2" t="s">
-        <v>18</v>
       </c>
     </row>
     <row r="3" spans="2:14" x14ac:dyDescent="0.25">

</xml_diff>